<commit_message>
Refactor layout and styling across various components for improved responsiveness and user experience. Adjusted padding, margins, and font sizes in card, list, practice, and feedback components. Added Hebrew translations for feedback form and improved accessibility features.
</commit_message>
<xml_diff>
--- a/public/questions_template.xlsx
+++ b/public/questions_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raph\projects\gifted-v3\smarti-web\smarti-web\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DED54C-1BDB-4A7B-88BF-D80D272D5B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC09FF3-4DFC-4288-83A6-CF88A25EBFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-150" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add managerId field to Question model and update related components for question management
</commit_message>
<xml_diff>
--- a/public/questions_template.xlsx
+++ b/public/questions_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raph\projects\gifted-v3\smarti-web\smarti-web\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC09FF3-4DFC-4288-83A6-CF88A25EBFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE93B1F9-AB81-4EFB-8846-7D3F8737F980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-150" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>content</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>תרגול במתמטיקה</t>
+  </si>
+  <si>
+    <t>managerId</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +494,7 @@
     <col min="8" max="8" width="65.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,8 +525,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -554,8 +560,11 @@
       <c r="J2" t="s">
         <v>31</v>
       </c>
+      <c r="K2">
+        <v>123</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -586,8 +595,11 @@
       <c r="J3" t="s">
         <v>32</v>
       </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -617,6 +629,9 @@
       </c>
       <c r="J4" t="s">
         <v>33</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>